<commit_message>
new asm test case
</commit_message>
<xml_diff>
--- a/MicroCPUInstructionWord.xlsx
+++ b/MicroCPUInstructionWord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbs/src/CPUKit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbs/src/Kartana9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15C91C61-4B5B-9247-8203-CB37DA2AB2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0292E661-B544-D34E-AD25-2BD0329F5666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33640" windowHeight="21580" xr2:uid="{1A9992FB-C001-7647-8C04-DC19BDE12C33}"/>
+    <workbookView xWindow="6280" yWindow="760" windowWidth="33640" windowHeight="21580" xr2:uid="{1A9992FB-C001-7647-8C04-DC19BDE12C33}"/>
   </bookViews>
   <sheets>
     <sheet name="MainInstructionCard" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="413">
   <si>
     <t>Instruction Word</t>
   </si>
@@ -1272,6 +1272,15 @@
   </si>
   <si>
     <t>Mneumonic Fmt</t>
+  </si>
+  <si>
+    <t>CMPI</t>
+  </si>
+  <si>
+    <t>CMPI a,#imm16</t>
+  </si>
+  <si>
+    <t>Potential new instruction</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1420,7 @@
       <name val="IBM Plex Mono Regular"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1528,6 +1537,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2326,7 +2347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="268">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2813,6 +2834,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3140,7 +3177,7 @@
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2640" activePane="bottomLeft"/>
       <selection activeCell="AF3" sqref="AF1:AF1048576"/>
-      <selection pane="bottomLeft" activeCell="M136" sqref="M136:N136"/>
+      <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6463,7 +6500,7 @@
         <v>61</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L21" s="17"/>
       <c r="M21" s="17" t="s">
@@ -7037,8 +7074,8 @@
         <f t="shared" si="6"/>
         <v>0010000</v>
       </c>
-      <c r="I25" s="34" t="s">
-        <v>19</v>
+      <c r="I25" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="J25" s="39" t="s">
         <v>61</v>
@@ -7461,8 +7498,8 @@
         <f t="shared" si="6"/>
         <v>0010010</v>
       </c>
-      <c r="I27" s="34" t="s">
-        <v>19</v>
+      <c r="I27" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="J27" s="39" t="s">
         <v>61</v>
@@ -8548,11 +8585,15 @@
         <f t="shared" si="6"/>
         <v>0011000</v>
       </c>
-      <c r="I33" s="34"/>
+      <c r="I33" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J33" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K33" s="17"/>
+      <c r="K33" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17" t="s">
         <v>347</v>
@@ -8756,11 +8797,15 @@
         <f t="shared" si="6"/>
         <v>0011001</v>
       </c>
-      <c r="I34" s="34"/>
+      <c r="I34" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J34" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K34" s="17"/>
+      <c r="K34" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L34" s="17"/>
       <c r="M34" s="17" t="s">
         <v>348</v>
@@ -8964,11 +9009,15 @@
         <f t="shared" si="6"/>
         <v>0011010</v>
       </c>
-      <c r="I35" s="34"/>
+      <c r="I35" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J35" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K35" s="17"/>
+      <c r="K35" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L35" s="17"/>
       <c r="M35" s="17" t="s">
         <v>349</v>
@@ -9172,11 +9221,15 @@
         <f t="shared" si="6"/>
         <v>0011011</v>
       </c>
-      <c r="I36" s="34"/>
+      <c r="I36" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J36" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K36" s="17"/>
+      <c r="K36" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L36" s="17"/>
       <c r="M36" s="17" t="s">
         <v>350</v>
@@ -9380,11 +9433,15 @@
         <f t="shared" si="6"/>
         <v>0011100</v>
       </c>
-      <c r="I37" s="34"/>
+      <c r="I37" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J37" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K37" s="17"/>
+      <c r="K37" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17" t="s">
         <v>351</v>
@@ -9589,13 +9646,13 @@
         <v>0011101</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J38" s="39" t="s">
         <v>61</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L38" s="17" t="s">
         <v>19</v>
@@ -9802,11 +9859,15 @@
         <f t="shared" si="6"/>
         <v>0011110</v>
       </c>
-      <c r="I39" s="34"/>
+      <c r="I39" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J39" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K39" s="17"/>
+      <c r="K39" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L39" s="18"/>
       <c r="M39" s="17" t="s">
         <v>353</v>
@@ -11694,8 +11755,12 @@
       <c r="I51" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="J51" s="36"/>
-      <c r="K51" s="17"/>
+      <c r="J51" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K51" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L51" s="17"/>
       <c r="M51" s="17" t="s">
         <v>358</v>
@@ -11897,11 +11962,15 @@
         <f t="shared" si="6"/>
         <v>0101011</v>
       </c>
-      <c r="I52" s="34"/>
+      <c r="I52" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J52" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K52" s="17"/>
+      <c r="K52" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L52" s="17"/>
       <c r="M52" s="17" t="s">
         <v>359</v>
@@ -12109,7 +12178,9 @@
       <c r="J53" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K53" s="17"/>
+      <c r="K53" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L53" s="17"/>
       <c r="M53" s="17" t="s">
         <v>360</v>
@@ -12311,9 +12382,15 @@
         <f t="shared" si="6"/>
         <v>0101101</v>
       </c>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="17"/>
+      <c r="I54" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17" t="s">
         <v>361</v>
@@ -12515,11 +12592,15 @@
         <f t="shared" si="6"/>
         <v>0101110</v>
       </c>
-      <c r="I55" s="34"/>
+      <c r="I55" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="J55" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K55" s="17"/>
+      <c r="K55" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="L55" s="17"/>
       <c r="M55" s="17" t="s">
         <v>362</v>
@@ -12843,7 +12924,9 @@
         <v>62</v>
       </c>
       <c r="J57" s="41"/>
-      <c r="K57" s="14"/>
+      <c r="K57" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="L57" s="140"/>
       <c r="M57" s="178" t="s">
         <v>363</v>
@@ -13229,7 +13312,9 @@
       </c>
       <c r="I59" s="42"/>
       <c r="J59" s="41"/>
-      <c r="K59" s="14"/>
+      <c r="K59" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="L59" s="15"/>
       <c r="M59" s="14"/>
       <c r="N59" s="15"/>
@@ -13583,11 +13668,15 @@
         <f t="shared" si="6"/>
         <v>0110100</v>
       </c>
-      <c r="I62" s="42"/>
+      <c r="I62" s="44" t="s">
+        <v>24</v>
+      </c>
       <c r="J62" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="K62" s="14"/>
+      <c r="K62" s="270" t="s">
+        <v>24</v>
+      </c>
       <c r="L62" s="140"/>
       <c r="M62" s="264" t="s">
         <v>364</v>
@@ -13972,13 +14061,13 @@
         <v>0110101</v>
       </c>
       <c r="I64" s="44" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J64" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="K64" s="16" t="s">
-        <v>19</v>
+      <c r="K64" s="270" t="s">
+        <v>24</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="14"/>
@@ -14464,11 +14553,13 @@
         <v>0111000</v>
       </c>
       <c r="I68" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="J68" s="41"/>
-      <c r="K68" s="16" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="J68" s="271" t="s">
+        <v>24</v>
+      </c>
+      <c r="K68" s="270" t="s">
+        <v>24</v>
       </c>
       <c r="L68" s="140"/>
       <c r="M68" s="178" t="s">
@@ -15931,9 +16022,15 @@
         <f t="shared" si="13"/>
         <v>1000010</v>
       </c>
-      <c r="I79" s="24"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="24"/>
+      <c r="I79" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J79" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K79" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L79" s="24" t="s">
         <v>124</v>
       </c>
@@ -16137,9 +16234,15 @@
         <f t="shared" si="13"/>
         <v>1000011</v>
       </c>
-      <c r="I80" s="24"/>
-      <c r="J80" s="24"/>
-      <c r="K80" s="24"/>
+      <c r="I80" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J80" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K80" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L80" s="24" t="s">
         <v>124</v>
       </c>
@@ -16341,11 +16444,15 @@
         <f t="shared" si="13"/>
         <v>1000100</v>
       </c>
-      <c r="I81" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J81" s="24"/>
-      <c r="K81" s="24"/>
+      <c r="I81" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J81" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K81" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L81" s="24" t="s">
         <v>124</v>
       </c>
@@ -16549,11 +16656,15 @@
         <f t="shared" si="13"/>
         <v>1000101</v>
       </c>
-      <c r="I82" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J82" s="24"/>
-      <c r="K82" s="24"/>
+      <c r="I82" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J82" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K82" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L82" s="24" t="s">
         <v>124</v>
       </c>
@@ -16755,11 +16866,15 @@
         <f t="shared" si="13"/>
         <v>1000110</v>
       </c>
-      <c r="I83" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J83" s="24"/>
-      <c r="K83" s="24"/>
+      <c r="I83" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J83" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K83" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L83" s="24" t="s">
         <v>124</v>
       </c>
@@ -17081,11 +17196,15 @@
         <f t="shared" si="13"/>
         <v>1001000</v>
       </c>
-      <c r="I85" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J85" s="24"/>
-      <c r="K85" s="24"/>
+      <c r="I85" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J85" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K85" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L85" s="24" t="s">
         <v>124</v>
       </c>
@@ -17407,11 +17526,15 @@
         <f t="shared" si="13"/>
         <v>1001010</v>
       </c>
-      <c r="I87" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J87" s="24"/>
-      <c r="K87" s="24"/>
+      <c r="I87" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J87" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K87" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L87" s="24" t="s">
         <v>124</v>
       </c>
@@ -18225,9 +18348,11 @@
         <f t="shared" si="13"/>
         <v>1010000</v>
       </c>
-      <c r="I93" s="24"/>
-      <c r="J93" s="24" t="s">
-        <v>19</v>
+      <c r="I93" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J93" s="268" t="s">
+        <v>24</v>
       </c>
       <c r="K93" s="24" t="s">
         <v>60</v>
@@ -18437,9 +18562,11 @@
         <f t="shared" si="13"/>
         <v>1010001</v>
       </c>
-      <c r="I94" s="24"/>
-      <c r="J94" s="24" t="s">
-        <v>19</v>
+      <c r="I94" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J94" s="268" t="s">
+        <v>24</v>
       </c>
       <c r="K94" s="24" t="s">
         <v>60</v>
@@ -18655,11 +18782,17 @@
       <c r="J95" s="24"/>
       <c r="K95" s="24"/>
       <c r="L95" s="21"/>
-      <c r="M95" s="24"/>
-      <c r="N95" s="21"/>
+      <c r="M95" s="272" t="s">
+        <v>410</v>
+      </c>
+      <c r="N95" s="273" t="s">
+        <v>411</v>
+      </c>
       <c r="O95" s="21"/>
       <c r="P95" s="21"/>
-      <c r="Q95" s="21"/>
+      <c r="Q95" s="273" t="s">
+        <v>412</v>
+      </c>
       <c r="R95" s="83"/>
       <c r="S95" s="82" t="s">
         <v>19</v>
@@ -18902,8 +19035,12 @@
       <c r="I97" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J97" s="24"/>
-      <c r="K97" s="24"/>
+      <c r="J97" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K97" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L97" s="24" t="s">
         <v>124</v>
       </c>
@@ -19110,8 +19247,12 @@
       <c r="I98" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J98" s="24"/>
-      <c r="K98" s="24"/>
+      <c r="J98" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K98" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L98" s="24" t="s">
         <v>124</v>
       </c>
@@ -19554,9 +19695,15 @@
         <f t="shared" si="13"/>
         <v>1011000</v>
       </c>
-      <c r="I101" s="24"/>
-      <c r="J101" s="24"/>
-      <c r="K101" s="24"/>
+      <c r="I101" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J101" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L101" s="24" t="s">
         <v>124</v>
       </c>
@@ -19762,9 +19909,15 @@
         <f t="shared" si="13"/>
         <v>1011001</v>
       </c>
-      <c r="I102" s="24"/>
-      <c r="J102" s="24"/>
-      <c r="K102" s="24"/>
+      <c r="I102" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J102" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K102" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L102" s="24" t="s">
         <v>124</v>
       </c>
@@ -19970,9 +20123,15 @@
         <f t="shared" si="13"/>
         <v>1011010</v>
       </c>
-      <c r="I103" s="24"/>
-      <c r="J103" s="24"/>
-      <c r="K103" s="24"/>
+      <c r="I103" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J103" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K103" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L103" s="24" t="s">
         <v>124</v>
       </c>
@@ -20178,9 +20337,15 @@
         <f t="shared" si="13"/>
         <v>1011011</v>
       </c>
-      <c r="I104" s="24"/>
-      <c r="J104" s="24"/>
-      <c r="K104" s="24"/>
+      <c r="I104" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J104" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K104" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L104" s="24" t="s">
         <v>124</v>
       </c>
@@ -20386,9 +20551,15 @@
         <f t="shared" si="13"/>
         <v>1011100</v>
       </c>
-      <c r="I105" s="24"/>
-      <c r="J105" s="24"/>
-      <c r="K105" s="24"/>
+      <c r="I105" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J105" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K105" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L105" s="24" t="s">
         <v>124</v>
       </c>
@@ -20594,9 +20765,15 @@
         <f t="shared" si="13"/>
         <v>1011101</v>
       </c>
-      <c r="I106" s="24"/>
-      <c r="J106" s="24"/>
-      <c r="K106" s="24"/>
+      <c r="I106" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J106" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K106" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L106" s="24" t="s">
         <v>124</v>
       </c>
@@ -20802,9 +20979,15 @@
         <f t="shared" si="13"/>
         <v>1011110</v>
       </c>
-      <c r="I107" s="24"/>
-      <c r="J107" s="24"/>
-      <c r="K107" s="24"/>
+      <c r="I107" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J107" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K107" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L107" s="24" t="s">
         <v>124</v>
       </c>
@@ -21137,8 +21320,12 @@
         <f t="shared" si="13"/>
         <v>1100000</v>
       </c>
-      <c r="I109" s="24"/>
-      <c r="J109" s="24"/>
+      <c r="I109" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J109" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="K109" s="24" t="s">
         <v>60</v>
       </c>
@@ -21347,8 +21534,12 @@
         <f t="shared" si="13"/>
         <v>1100001</v>
       </c>
-      <c r="I110" s="24"/>
-      <c r="J110" s="24"/>
+      <c r="I110" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="J110" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="K110" s="24" t="s">
         <v>60</v>
       </c>
@@ -21796,8 +21987,12 @@
       <c r="I113" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J113" s="24"/>
-      <c r="K113" s="24"/>
+      <c r="J113" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K113" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L113" s="24" t="s">
         <v>124</v>
       </c>
@@ -22006,8 +22201,12 @@
       <c r="I114" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J114" s="24"/>
-      <c r="K114" s="24"/>
+      <c r="J114" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K114" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L114" s="24" t="s">
         <v>124</v>
       </c>
@@ -22216,8 +22415,12 @@
       <c r="I115" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J115" s="24"/>
-      <c r="K115" s="24"/>
+      <c r="J115" s="268" t="s">
+        <v>24</v>
+      </c>
+      <c r="K115" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L115" s="24" t="s">
         <v>124</v>
       </c>
@@ -22541,7 +22744,9 @@
       </c>
       <c r="I117" s="24"/>
       <c r="J117" s="24"/>
-      <c r="K117" s="24"/>
+      <c r="K117" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L117" s="24" t="s">
         <v>124</v>
       </c>
@@ -22749,7 +22954,9 @@
       </c>
       <c r="I118" s="24"/>
       <c r="J118" s="24"/>
-      <c r="K118" s="24"/>
+      <c r="K118" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L118" s="24" t="s">
         <v>124</v>
       </c>
@@ -22957,7 +23164,9 @@
       </c>
       <c r="I119" s="24"/>
       <c r="J119" s="24"/>
-      <c r="K119" s="24"/>
+      <c r="K119" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L119" s="24" t="s">
         <v>124</v>
       </c>
@@ -23165,7 +23374,9 @@
       </c>
       <c r="I120" s="24"/>
       <c r="J120" s="24"/>
-      <c r="K120" s="24"/>
+      <c r="K120" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L120" s="24" t="s">
         <v>124</v>
       </c>
@@ -23373,7 +23584,9 @@
       </c>
       <c r="I121" s="24"/>
       <c r="J121" s="24"/>
-      <c r="K121" s="24"/>
+      <c r="K121" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L121" s="24" t="s">
         <v>124</v>
       </c>
@@ -23581,7 +23794,9 @@
       </c>
       <c r="I122" s="24"/>
       <c r="J122" s="24"/>
-      <c r="K122" s="24"/>
+      <c r="K122" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L122" s="24" t="s">
         <v>124</v>
       </c>
@@ -23789,7 +24004,9 @@
       </c>
       <c r="I123" s="24"/>
       <c r="J123" s="24"/>
-      <c r="K123" s="24"/>
+      <c r="K123" s="268" t="s">
+        <v>24</v>
+      </c>
       <c r="L123" s="24" t="s">
         <v>124</v>
       </c>
@@ -24944,7 +25161,9 @@
       </c>
       <c r="I132" s="66"/>
       <c r="J132" s="66"/>
-      <c r="K132" s="66"/>
+      <c r="K132" s="269" t="s">
+        <v>24</v>
+      </c>
       <c r="L132" s="195" t="s">
         <v>124</v>
       </c>
@@ -25193,7 +25412,9 @@
       </c>
       <c r="I134" s="66"/>
       <c r="J134" s="66"/>
-      <c r="K134" s="66"/>
+      <c r="K134" s="269" t="s">
+        <v>24</v>
+      </c>
       <c r="L134" s="197" t="s">
         <v>124</v>
       </c>
@@ -25388,7 +25609,9 @@
       </c>
       <c r="I135" s="66"/>
       <c r="J135" s="66"/>
-      <c r="K135" s="66"/>
+      <c r="K135" s="269" t="s">
+        <v>24</v>
+      </c>
       <c r="L135" s="198" t="s">
         <v>229</v>
       </c>
@@ -25587,7 +25810,9 @@
       </c>
       <c r="I136" s="66"/>
       <c r="J136" s="66"/>
-      <c r="K136" s="66"/>
+      <c r="K136" s="269" t="s">
+        <v>24</v>
+      </c>
       <c r="L136" s="197" t="s">
         <v>229</v>
       </c>
@@ -25782,7 +26007,9 @@
       </c>
       <c r="I137" s="66"/>
       <c r="J137" s="66"/>
-      <c r="K137" s="66"/>
+      <c r="K137" s="269" t="s">
+        <v>24</v>
+      </c>
       <c r="L137" s="198" t="s">
         <v>229</v>
       </c>
@@ -30511,6 +30738,7 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes to instruction naming
</commit_message>
<xml_diff>
--- a/MicroCPUInstructionWord.xlsx
+++ b/MicroCPUInstructionWord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbs/src/Kartana9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0292E661-B544-D34E-AD25-2BD0329F5666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A475F1D6-61BA-E141-9190-DCD10786EA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6280" yWindow="760" windowWidth="33640" windowHeight="21580" xr2:uid="{1A9992FB-C001-7647-8C04-DC19BDE12C33}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="421">
   <si>
     <t>Instruction Word</t>
   </si>
@@ -281,9 +281,6 @@
     <t>cnt</t>
   </si>
   <si>
-    <t>MOV SP,c</t>
-  </si>
-  <si>
     <t>MOV b,c</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>if NV: jmp to [b]</t>
   </si>
   <si>
-    <t>MOV b,SP</t>
-  </si>
-  <si>
     <t>CMP a,b</t>
   </si>
   <si>
@@ -455,9 +449,6 @@
     <t>JZ +imm16</t>
   </si>
   <si>
-    <t>jump to PC+imm16</t>
-  </si>
-  <si>
     <t>if Z jump to PC+imm16</t>
   </si>
   <si>
@@ -806,9 +797,6 @@
     <t>CF=LAST BIT</t>
   </si>
   <si>
-    <t>MOV PC,c</t>
-  </si>
-  <si>
     <t>BinOpCode</t>
   </si>
   <si>
@@ -1281,6 +1269,42 @@
   </si>
   <si>
     <t>Potential new instruction</t>
+  </si>
+  <si>
+    <t>MOVSP c</t>
+  </si>
+  <si>
+    <t>MOVTSP b</t>
+  </si>
+  <si>
+    <t>MOVPC c</t>
+  </si>
+  <si>
+    <t>JMPIO</t>
+  </si>
+  <si>
+    <t>JZRIO</t>
+  </si>
+  <si>
+    <t>JNZIO</t>
+  </si>
+  <si>
+    <t>JNCIO</t>
+  </si>
+  <si>
+    <t>JCIO</t>
+  </si>
+  <si>
+    <t>JVIO</t>
+  </si>
+  <si>
+    <t>JNVIO</t>
+  </si>
+  <si>
+    <t>jump to PC+imm16 offset</t>
+  </si>
+  <si>
+    <t>CALLIO</t>
   </si>
 </sst>
 </file>
@@ -3177,7 +3201,7 @@
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2640" activePane="bottomLeft"/>
       <selection activeCell="AF3" sqref="AF1:AF1048576"/>
-      <selection pane="bottomLeft" activeCell="Q95" sqref="Q95"/>
+      <selection pane="bottomLeft" activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3245,7 +3269,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
       <c r="Z2" s="249" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AA2" s="250"/>
       <c r="AB2" s="250"/>
@@ -3277,13 +3301,13 @@
       <c r="BB2" s="250"/>
       <c r="BC2" s="250"/>
       <c r="BE2" s="247" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="BF2" s="247"/>
       <c r="BG2" s="247"/>
       <c r="BH2" s="247"/>
       <c r="BJ2" s="247" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="BK2" s="247"/>
       <c r="BL2" s="248"/>
@@ -3291,25 +3315,25 @@
     </row>
     <row r="3" spans="2:91" s="25" customFormat="1" ht="110" customHeight="1">
       <c r="B3" s="109" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C3" s="109" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D3" s="109" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E3" s="109" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>64</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I3" s="109" t="s">
         <v>65</v>
@@ -3323,61 +3347,61 @@
       <c r="L3" s="26"/>
       <c r="M3" s="109"/>
       <c r="S3" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="T3" s="93" t="s">
+        <v>148</v>
+      </c>
+      <c r="U3" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="V3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="93" t="s">
+      <c r="W3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="U3" s="93" t="s">
-        <v>152</v>
-      </c>
-      <c r="V3" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="W3" s="26" t="s">
+      <c r="X3" s="26" t="s">
         <v>154</v>
-      </c>
-      <c r="X3" s="26" t="s">
-        <v>157</v>
       </c>
       <c r="Y3" s="26" t="s">
         <v>19</v>
       </c>
       <c r="Z3" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AA3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC3" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF3" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH3" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ3" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="AB3" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC3" s="26" t="s">
-        <v>332</v>
-      </c>
-      <c r="AD3" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="AE3" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="AF3" s="26" t="s">
+      <c r="AK3" s="26" t="s">
         <v>170</v>
-      </c>
-      <c r="AG3" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH3" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="AI3" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="AJ3" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="AK3" s="26" t="s">
-        <v>173</v>
       </c>
       <c r="AL3" s="26" t="s">
         <v>18</v>
@@ -3386,75 +3410,75 @@
         <v>33</v>
       </c>
       <c r="AN3" s="26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AO3" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AP3" s="26" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AQ3" s="26" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AR3" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AS3" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AT3" s="26" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AU3" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AV3" s="26"/>
       <c r="AW3" s="26"/>
       <c r="AX3" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AY3" s="26" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AZ3" s="26" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="BA3" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="BB3" s="26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BD3" s="26" t="s">
         <v>19</v>
       </c>
       <c r="BE3" s="26" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="BF3" s="26" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="BG3" s="26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="BH3" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="BI3" s="26" t="s">
         <v>19</v>
       </c>
       <c r="BJ3" s="26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="BK3" s="26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="BL3" s="26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="BM3" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="BN3" s="26" t="s">
         <v>19</v>
@@ -3623,7 +3647,7 @@
     </row>
     <row r="5" spans="2:91" s="27" customFormat="1" ht="20" customHeight="1" thickBot="1">
       <c r="B5" s="245" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C5" s="246"/>
       <c r="D5" s="184"/>
@@ -3645,7 +3669,7 @@
       <c r="T5" s="98"/>
       <c r="U5" s="101"/>
       <c r="V5" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W5" s="68">
         <v>16</v>
@@ -3782,7 +3806,7 @@
     </row>
     <row r="6" spans="2:91" s="27" customFormat="1" ht="20" customHeight="1" thickBot="1">
       <c r="B6" s="182" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C6" s="183"/>
       <c r="D6" s="184"/>
@@ -3804,7 +3828,7 @@
       <c r="T6" s="98"/>
       <c r="U6" s="101"/>
       <c r="V6" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W6" s="68">
         <v>16</v>
@@ -4032,32 +4056,32 @@
         <v>15</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G8" s="139" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H8" s="139"/>
       <c r="I8" s="54" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K8" s="53" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M8" s="55" t="s">
         <v>1</v>
       </c>
       <c r="N8" s="58" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="O8" s="59" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="P8" s="59"/>
       <c r="Q8" s="59" t="s">
@@ -4073,7 +4097,7 @@
         <v>19</v>
       </c>
       <c r="U8" s="94" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="V8" s="94"/>
       <c r="W8" s="67"/>
@@ -4191,7 +4215,7 @@
         <v>2</v>
       </c>
       <c r="O9" s="204" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P9" s="204" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O9," (SM_EX1 &amp; opcf:['b'",H9,"])")</f>
@@ -4205,14 +4229,14 @@
       </c>
       <c r="S9" s="206"/>
       <c r="T9" s="205" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U9" s="207" t="str">
         <f>_xlfn.CONCAT(MID(DEC2BIN(B9,8),3,2)," ",MID(DEC2BIN(B9,8),5,3))</f>
         <v>00 000</v>
       </c>
       <c r="V9" s="95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
@@ -4393,32 +4417,32 @@
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="P10" s="18" t="str">
         <f t="shared" ref="P10:P15" si="4">_xlfn.CONCAT("$DEFINE ",O10," (SM_EX1 &amp; opcf:['b'",H10,"])")</f>
         <v>$DEFINE INST_HALT (SM_EX1 &amp; opcf:['b'0000001])</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="R10" s="75"/>
       <c r="S10" s="74"/>
       <c r="T10" s="75" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U10" s="208" t="str">
         <f t="shared" ref="U10:U77" si="5">_xlfn.CONCAT(MID(DEC2BIN(B10,8),3,2)," ",MID(DEC2BIN(B10,8),5,3))</f>
         <v>00 000</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W10" s="68"/>
       <c r="X10" s="68"/>
@@ -4597,13 +4621,13 @@
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="17" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="N11" s="18" t="s">
         <v>8</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P11" s="18" t="str">
         <f t="shared" si="4"/>
@@ -4613,20 +4637,20 @@
         <v>12</v>
       </c>
       <c r="R11" s="75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T11" s="75" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U11" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 001</v>
       </c>
       <c r="V11" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W11" s="68"/>
       <c r="X11" s="68"/>
@@ -4807,13 +4831,13 @@
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="P12" s="18" t="str">
         <f t="shared" si="4"/>
@@ -4821,20 +4845,20 @@
       </c>
       <c r="Q12" s="18"/>
       <c r="R12" s="75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S12" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T12" s="75" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U12" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 001</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W12" s="68"/>
       <c r="X12" s="68"/>
@@ -5015,13 +5039,13 @@
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="17" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="N13" s="18" t="s">
         <v>6</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="P13" s="18" t="str">
         <f t="shared" si="4"/>
@@ -5031,20 +5055,20 @@
         <v>7</v>
       </c>
       <c r="R13" s="75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S13" s="74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T13" s="75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U13" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 010</v>
       </c>
       <c r="V13" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W13" s="68"/>
       <c r="X13" s="68"/>
@@ -5225,13 +5249,13 @@
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="17" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="P14" s="18" t="str">
         <f t="shared" si="4"/>
@@ -5239,20 +5263,20 @@
       </c>
       <c r="Q14" s="18"/>
       <c r="R14" s="75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S14" s="74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T14" s="75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U14" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 010</v>
       </c>
       <c r="V14" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W14" s="68"/>
       <c r="X14" s="68"/>
@@ -5439,7 +5463,7 @@
         <v>11</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="P15" s="18" t="str">
         <f t="shared" si="4"/>
@@ -5449,20 +5473,20 @@
         <v>16</v>
       </c>
       <c r="R15" s="75" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S15" s="74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T15" s="75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U15" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 011</v>
       </c>
       <c r="V15" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W15" s="68"/>
       <c r="X15" s="68"/>
@@ -5650,7 +5674,7 @@
       <c r="R16" s="75"/>
       <c r="S16" s="74"/>
       <c r="T16" s="75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U16" s="208" t="str">
         <f t="shared" si="5"/>
@@ -5774,7 +5798,7 @@
         <v>10</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P17" s="18" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O17," (SM_EX1 &amp; opcf:['b'",H17,"])")</f>
@@ -5784,20 +5808,20 @@
         <v>15</v>
       </c>
       <c r="R17" s="75" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S17" s="74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T17" s="75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U17" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 100</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W17" s="68"/>
       <c r="X17" s="68"/>
@@ -5985,7 +6009,7 @@
       <c r="R18" s="75"/>
       <c r="S18" s="74"/>
       <c r="T18" s="75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U18" s="208" t="str">
         <f t="shared" si="5"/>
@@ -6111,7 +6135,7 @@
         <v>9</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P19" s="18" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O19," (SM_EX1 &amp; opcf:['b'",H19,"])")</f>
@@ -6121,20 +6145,20 @@
         <v>14</v>
       </c>
       <c r="R19" s="75" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S19" s="74" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T19" s="75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U19" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 101</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W19" s="68"/>
       <c r="X19" s="68"/>
@@ -6322,7 +6346,7 @@
         <v>58</v>
       </c>
       <c r="T20" s="75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U20" s="208" t="str">
         <f t="shared" si="5"/>
@@ -6504,13 +6528,13 @@
       </c>
       <c r="L21" s="17"/>
       <c r="M21" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="N21" s="18" t="s">
         <v>57</v>
       </c>
       <c r="O21" s="18" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="P21" s="18" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O21," (SM_EX1 &amp; opcf:['b'",H21,"])")</f>
@@ -6520,20 +6544,20 @@
         <v>17</v>
       </c>
       <c r="R21" s="75" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S21" s="74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T21" s="75" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U21" s="208" t="str">
         <f t="shared" si="5"/>
         <v>00 110</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W21" s="68"/>
       <c r="X21" s="68"/>
@@ -6723,7 +6747,7 @@
         <v>58</v>
       </c>
       <c r="T22" s="75" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U22" s="208" t="str">
         <f t="shared" si="5"/>
@@ -6852,7 +6876,7 @@
         <v>58</v>
       </c>
       <c r="T23" s="75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U23" s="208" t="str">
         <f t="shared" si="5"/>
@@ -6967,7 +6991,7 @@
         <v>58</v>
       </c>
       <c r="T24" s="75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U24" s="208" t="str">
         <f t="shared" si="5"/>
@@ -7085,13 +7109,13 @@
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="N25" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O25" s="18" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="P25" s="18" t="str">
         <f t="shared" ref="P25:P30" si="8">_xlfn.CONCAT("$DEFINE ",O25," (SM_EX1 &amp; opcf:['b'",H25,"])")</f>
@@ -7104,17 +7128,17 @@
         <v>58</v>
       </c>
       <c r="S25" s="72" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T25" s="73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U25" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 000</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W25" s="68">
         <v>16</v>
@@ -7297,13 +7321,13 @@
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="17" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="N26" s="18" t="s">
         <v>74</v>
       </c>
       <c r="O26" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P26" s="18" t="str">
         <f t="shared" si="8"/>
@@ -7316,17 +7340,17 @@
         <v>58</v>
       </c>
       <c r="S26" s="74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T26" s="75" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U26" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 000</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W26" s="68">
         <v>8</v>
@@ -7405,13 +7429,13 @@
         <v>1</v>
       </c>
       <c r="AY26" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ26" s="104">
         <v>0</v>
       </c>
       <c r="BA26" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB26" s="104">
         <v>0</v>
@@ -7425,10 +7449,10 @@
         <v>0</v>
       </c>
       <c r="BG26" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH26" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI26" s="60"/>
       <c r="BJ26" s="106">
@@ -7509,36 +7533,36 @@
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="P27" s="18" t="str">
         <f t="shared" si="8"/>
         <v>$DEFINE INST_CMP_A_B (SM_EX1 &amp; opcf:['b'0010010])</v>
       </c>
       <c r="Q27" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R27" s="75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S27" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T27" s="75" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U27" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 001</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W27" s="68"/>
       <c r="X27" s="68"/>
@@ -7719,29 +7743,29 @@
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="P28" s="18" t="str">
         <f t="shared" si="8"/>
         <v>$DEFINE INST_CMPC (SM_EX1 &amp; opcf:['b'0010011])</v>
       </c>
       <c r="Q28" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R28" s="75" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S28" s="74" t="s">
         <v>58</v>
       </c>
       <c r="T28" s="75" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U28" s="208" t="str">
         <f t="shared" si="5"/>
@@ -7923,13 +7947,13 @@
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="N29" s="18" t="s">
         <v>71</v>
       </c>
       <c r="O29" s="18" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="P29" s="18" t="str">
         <f t="shared" si="8"/>
@@ -7945,14 +7969,14 @@
         <v>58</v>
       </c>
       <c r="T29" s="75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U29" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 010</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W29" s="68">
         <v>16</v>
@@ -8135,13 +8159,13 @@
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="N30" s="18" t="s">
         <v>70</v>
       </c>
       <c r="O30" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="P30" s="18" t="str">
         <f t="shared" si="8"/>
@@ -8157,14 +8181,14 @@
         <v>58</v>
       </c>
       <c r="T30" s="75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U30" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 010</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W30" s="68">
         <v>8</v>
@@ -8243,13 +8267,13 @@
         <v>1</v>
       </c>
       <c r="AY30" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ30" s="106">
         <v>1</v>
       </c>
       <c r="BA30" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB30" s="106">
         <v>1</v>
@@ -8263,10 +8287,10 @@
         <v>0</v>
       </c>
       <c r="BG30" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH30" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI30" s="60"/>
       <c r="BJ30" s="106">
@@ -8358,7 +8382,7 @@
         <v>58</v>
       </c>
       <c r="T31" s="75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U31" s="208" t="str">
         <f t="shared" si="5"/>
@@ -8481,7 +8505,7 @@
         <v>58</v>
       </c>
       <c r="T32" s="75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U32" s="208" t="str">
         <f t="shared" si="5"/>
@@ -8596,20 +8620,20 @@
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="N33" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O33" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P33" s="18" t="str">
         <f t="shared" ref="P33:P39" si="9">_xlfn.CONCAT("$DEFINE ",O33," (SM_EX1 &amp; opcf:['b'",H33,"])")</f>
         <v>$DEFINE INST_JMP_INDB (SM_EX1 &amp; opcf:['b'0011000])</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R33" s="75" t="s">
         <v>58</v>
@@ -8618,14 +8642,14 @@
         <v>58</v>
       </c>
       <c r="T33" s="75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U33" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 100</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W33" s="68"/>
       <c r="X33" s="70" t="s">
@@ -8808,20 +8832,20 @@
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="17" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="N34" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P34" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JZ_INDB (SM_EX1 &amp; opcf:['b'0011001])</v>
       </c>
       <c r="Q34" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R34" s="75" t="s">
         <v>58</v>
@@ -8830,14 +8854,14 @@
         <v>58</v>
       </c>
       <c r="T34" s="75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U34" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 100</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W34" s="68"/>
       <c r="X34" s="70" t="s">
@@ -9020,20 +9044,20 @@
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="17" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="N35" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="P35" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JNZ_INDB (SM_EX1 &amp; opcf:['b'0011010])</v>
       </c>
       <c r="Q35" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R35" s="75" t="s">
         <v>58</v>
@@ -9042,14 +9066,14 @@
         <v>58</v>
       </c>
       <c r="T35" s="75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U35" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 101</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W35" s="68"/>
       <c r="X35" s="70" t="s">
@@ -9232,20 +9256,20 @@
       </c>
       <c r="L36" s="17"/>
       <c r="M36" s="17" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="N36" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O36" s="18" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="P36" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JC_INDB (SM_EX1 &amp; opcf:['b'0011011])</v>
       </c>
       <c r="Q36" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R36" s="75" t="s">
         <v>58</v>
@@ -9254,14 +9278,14 @@
         <v>58</v>
       </c>
       <c r="T36" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U36" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 101</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W36" s="68"/>
       <c r="X36" s="70" t="s">
@@ -9444,20 +9468,20 @@
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="N37" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="P37" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JNC_INDB (SM_EX1 &amp; opcf:['b'0011100])</v>
       </c>
       <c r="Q37" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R37" s="75" t="s">
         <v>58</v>
@@ -9466,14 +9490,14 @@
         <v>58</v>
       </c>
       <c r="T37" s="75" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U37" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 110</v>
       </c>
       <c r="V37" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W37" s="68"/>
       <c r="X37" s="70" t="s">
@@ -9658,20 +9682,20 @@
         <v>19</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="N38" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P38" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JV_INDB (SM_EX1 &amp; opcf:['b'0011101])</v>
       </c>
       <c r="Q38" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R38" s="75" t="s">
         <v>58</v>
@@ -9680,14 +9704,14 @@
         <v>58</v>
       </c>
       <c r="T38" s="75" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U38" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 110</v>
       </c>
       <c r="V38" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W38" s="68"/>
       <c r="X38" s="70" t="s">
@@ -9870,20 +9894,20 @@
       </c>
       <c r="L39" s="18"/>
       <c r="M39" s="17" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="N39" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O39" s="18" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="P39" s="18" t="str">
         <f t="shared" si="9"/>
         <v>$DEFINE INST_JNV_INDB (SM_EX1 &amp; opcf:['b'0011110])</v>
       </c>
       <c r="Q39" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R39" s="75" t="s">
         <v>58</v>
@@ -9892,14 +9916,14 @@
         <v>58</v>
       </c>
       <c r="T39" s="75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U39" s="208" t="str">
         <f t="shared" si="5"/>
         <v>01 111</v>
       </c>
       <c r="V39" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W39" s="68"/>
       <c r="X39" s="70" t="s">
@@ -10077,7 +10101,7 @@
       <c r="L40" s="18"/>
       <c r="M40" s="17"/>
       <c r="N40" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="O40" s="18"/>
       <c r="P40" s="18"/>
@@ -10087,7 +10111,7 @@
         <v>58</v>
       </c>
       <c r="T40" s="75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U40" s="208" t="str">
         <f t="shared" si="5"/>
@@ -10201,7 +10225,7 @@
       <c r="L41" s="18"/>
       <c r="M41" s="17"/>
       <c r="N41" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O41" s="18"/>
       <c r="P41" s="18"/>
@@ -10211,7 +10235,7 @@
         <v>58</v>
       </c>
       <c r="T41" s="77" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U41" s="208" t="str">
         <f t="shared" si="5"/>
@@ -10322,7 +10346,7 @@
       <c r="L42" s="18"/>
       <c r="M42" s="17"/>
       <c r="N42" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O42" s="18"/>
       <c r="P42" s="18"/>
@@ -10332,7 +10356,7 @@
         <v>58</v>
       </c>
       <c r="T42" s="77" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U42" s="208" t="str">
         <f t="shared" si="5"/>
@@ -10449,36 +10473,36 @@
       </c>
       <c r="L43" s="17"/>
       <c r="M43" s="17" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="N43" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O43" s="18" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="P43" s="18" t="str">
         <f t="shared" ref="P43:P46" si="10">_xlfn.CONCAT("$DEFINE ",O43," (SM_EX1 &amp; opcf:['b'",H43,"])")</f>
         <v>$DEFINE INST_SHL_B_C_CNT (SM_EX1 &amp; opcf:['b'0100010])</v>
       </c>
       <c r="Q43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="R43" s="75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S43" s="74" t="s">
         <v>58</v>
       </c>
       <c r="T43" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U43" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 001</v>
       </c>
       <c r="V43" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W43" s="68"/>
       <c r="X43" s="68"/>
@@ -10659,36 +10683,36 @@
       </c>
       <c r="L44" s="17"/>
       <c r="M44" s="17" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="N44" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="P44" s="18" t="str">
         <f t="shared" si="10"/>
         <v>$DEFINE INST_SHR_B_C_CNT (SM_EX1 &amp; opcf:['b'0100011])</v>
       </c>
       <c r="Q44" s="18" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="R44" s="75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S44" s="74" t="s">
         <v>58</v>
       </c>
       <c r="T44" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U44" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 001</v>
       </c>
       <c r="V44" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W44" s="68"/>
       <c r="X44" s="68"/>
@@ -10869,36 +10893,36 @@
       </c>
       <c r="L45" s="17"/>
       <c r="M45" s="17" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="N45" s="18" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O45" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P45" s="18" t="str">
         <f t="shared" si="10"/>
         <v>$DEFINE INST_SHLC_B_C_CNT (SM_EX1 &amp; opcf:['b'0100100])</v>
       </c>
       <c r="Q45" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="R45" s="75" t="s">
         <v>250</v>
       </c>
-      <c r="R45" s="75" t="s">
-        <v>253</v>
-      </c>
       <c r="S45" s="74" t="s">
         <v>58</v>
       </c>
       <c r="T45" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U45" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 010</v>
       </c>
       <c r="V45" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W45" s="68"/>
       <c r="X45" s="68"/>
@@ -11073,36 +11097,36 @@
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="N46" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O46" s="18" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="P46" s="18" t="str">
         <f t="shared" si="10"/>
         <v>$DEFINE INST_SHRA_B_C_CNT (SM_EX1 &amp; opcf:['b'0100101])</v>
       </c>
       <c r="Q46" s="20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="R46" s="75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S46" s="74" t="s">
         <v>58</v>
       </c>
       <c r="T46" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U46" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 010</v>
       </c>
       <c r="V46" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W46" s="68"/>
       <c r="X46" s="68"/>
@@ -11278,7 +11302,7 @@
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O47" s="18"/>
       <c r="P47" s="18"/>
@@ -11288,7 +11312,7 @@
         <v>58</v>
       </c>
       <c r="T47" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U47" s="208" t="str">
         <f t="shared" si="5"/>
@@ -11398,7 +11422,7 @@
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
       <c r="N48" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O48" s="18"/>
       <c r="P48" s="18"/>
@@ -11408,7 +11432,7 @@
         <v>58</v>
       </c>
       <c r="T48" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U48" s="208" t="str">
         <f t="shared" si="5"/>
@@ -11528,7 +11552,7 @@
         <v>58</v>
       </c>
       <c r="T49" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U49" s="208" t="str">
         <f t="shared" si="5"/>
@@ -11648,7 +11672,7 @@
         <v>58</v>
       </c>
       <c r="T50" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U50" s="208" t="str">
         <f t="shared" si="5"/>
@@ -11763,36 +11787,36 @@
       </c>
       <c r="L51" s="17"/>
       <c r="M51" s="17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="N51" s="18" t="s">
-        <v>79</v>
+        <v>409</v>
       </c>
       <c r="O51" s="18" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="P51" s="18" t="str">
         <f t="shared" ref="P51:P55" si="11">_xlfn.CONCAT("$DEFINE ",O51," (SM_EX1 &amp; opcf:['b'",H51,"])")</f>
         <v>$DEFINE INST_MOV_SP_C (SM_EX1 &amp; opcf:['b'0101010])</v>
       </c>
       <c r="Q51" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="R51" s="75" t="s">
         <v>13</v>
       </c>
       <c r="S51" s="74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T51" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U51" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 101</v>
       </c>
       <c r="V51" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W51" s="68"/>
       <c r="X51" s="68"/>
@@ -11973,36 +11997,36 @@
       </c>
       <c r="L52" s="17"/>
       <c r="M52" s="17" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="N52" s="18" t="s">
-        <v>120</v>
+        <v>410</v>
       </c>
       <c r="O52" s="18" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="P52" s="18" t="str">
         <f t="shared" si="11"/>
         <v>$DEFINE INST_MOV_B_SP (SM_EX1 &amp; opcf:['b'0101011])</v>
       </c>
       <c r="Q52" s="18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R52" s="75" t="s">
         <v>58</v>
       </c>
       <c r="S52" s="74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T52" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U52" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 101</v>
       </c>
       <c r="V52" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W52" s="68"/>
       <c r="X52" s="68"/>
@@ -12183,36 +12207,36 @@
       </c>
       <c r="L53" s="17"/>
       <c r="M53" s="17" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="N53" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O53" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="P53" s="18" t="str">
         <f t="shared" si="11"/>
         <v>$DEFINE INST_MOV_B_C (SM_EX1 &amp; opcf:['b'0101100])</v>
       </c>
       <c r="Q53" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R53" s="75" t="s">
         <v>13</v>
       </c>
       <c r="S53" s="74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T53" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U53" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 110</v>
       </c>
       <c r="V53" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W53" s="68"/>
       <c r="X53" s="68"/>
@@ -12393,20 +12417,20 @@
       </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="N54" s="18" t="s">
-        <v>254</v>
+        <v>411</v>
       </c>
       <c r="O54" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="P54" s="18" t="str">
         <f t="shared" si="11"/>
         <v>$DEFINE INST_MOV_PC_C (SM_EX1 &amp; opcf:['b'0101101])</v>
       </c>
       <c r="Q54" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R54" s="75" t="s">
         <v>13</v>
@@ -12415,14 +12439,14 @@
         <v>58</v>
       </c>
       <c r="T54" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U54" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 110</v>
       </c>
       <c r="V54" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W54" s="68"/>
       <c r="X54" s="68"/>
@@ -12603,13 +12627,13 @@
       </c>
       <c r="L55" s="17"/>
       <c r="M55" s="17" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="N55" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O55" s="18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="P55" s="18" t="str">
         <f t="shared" si="11"/>
@@ -12620,17 +12644,17 @@
         <v>58</v>
       </c>
       <c r="S55" s="74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T55" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U55" s="208" t="str">
         <f t="shared" si="5"/>
         <v>10 111</v>
       </c>
       <c r="V55" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W55" s="68">
         <v>16</v>
@@ -12816,7 +12840,7 @@
         <v>19</v>
       </c>
       <c r="T56" s="77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U56" s="208" t="str">
         <f t="shared" si="5"/>
@@ -12929,13 +12953,13 @@
       </c>
       <c r="L57" s="140"/>
       <c r="M57" s="178" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="N57" s="140" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O57" s="140" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="P57" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O57," (SM_EX1 &amp; opcf:['b'",H57,"])")</f>
@@ -12949,14 +12973,14 @@
         <v>58</v>
       </c>
       <c r="T57" s="143" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U57" s="209" t="str">
         <f>_xlfn.CONCAT(MID(DEC2BIN(B41,8),3,2)," ",MID(DEC2BIN(B41,8),5,3))</f>
         <v>10 000</v>
       </c>
       <c r="V57" s="144" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W57" s="145">
         <v>16</v>
@@ -13123,10 +13147,10 @@
       <c r="L58" s="153"/>
       <c r="M58" s="179"/>
       <c r="N58" s="153" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O58" s="140" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="P58" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O58," (SM_EX2 &amp; opcf:['b'",H58,"])")</f>
@@ -13326,7 +13350,7 @@
         <v>58</v>
       </c>
       <c r="T59" s="112" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U59" s="212" t="str">
         <f t="shared" si="5"/>
@@ -13444,7 +13468,7 @@
         <v>58</v>
       </c>
       <c r="T60" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U60" s="212" t="str">
         <f t="shared" si="5"/>
@@ -13564,7 +13588,7 @@
         <v>58</v>
       </c>
       <c r="T61" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U61" s="212" t="str">
         <f t="shared" si="5"/>
@@ -13679,13 +13703,13 @@
       </c>
       <c r="L62" s="140"/>
       <c r="M62" s="264" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="N62" s="265" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O62" s="140" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="P62" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O62," (SM_EX1 &amp; opcf:['b'",H62,"])")</f>
@@ -13696,17 +13720,17 @@
         <v>58</v>
       </c>
       <c r="S62" s="142" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T62" s="143" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U62" s="209" t="str">
         <f t="shared" si="5"/>
         <v>11 010</v>
       </c>
       <c r="V62" s="144" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W62" s="145">
         <v>16</v>
@@ -13873,10 +13897,10 @@
       <c r="L63" s="153"/>
       <c r="M63" s="179"/>
       <c r="N63" s="153" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O63" s="140" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="P63" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O63," (SM_EX2 &amp; opcf:['b'",H63,"])")</f>
@@ -13887,7 +13911,7 @@
         <v>58</v>
       </c>
       <c r="S63" s="155" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T63" s="156"/>
       <c r="U63" s="210"/>
@@ -14077,10 +14101,10 @@
       <c r="Q64" s="15"/>
       <c r="R64" s="211"/>
       <c r="S64" s="78" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T64" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U64" s="212" t="str">
         <f t="shared" si="5"/>
@@ -14199,24 +14223,24 @@
       <c r="L65" s="15"/>
       <c r="M65" s="14"/>
       <c r="N65" s="196" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O65" s="15" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="P65" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O65," (SM_EX1 &amp; opcf:['b'",H65,"])")</f>
         <v>$DEFINE INST_CALL_INDB (SM_EX1 &amp; opcf:['b'0110110])</v>
       </c>
       <c r="Q65" s="196" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R65" s="211"/>
       <c r="S65" s="78" t="s">
         <v>58</v>
       </c>
       <c r="T65" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U65" s="212" t="str">
         <f t="shared" si="5"/>
@@ -14316,17 +14340,17 @@
       <c r="L66" s="15"/>
       <c r="M66" s="14"/>
       <c r="N66" s="196" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O66" s="15" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="P66" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O66," (SM_EX2 &amp; opcf:['b'",H66,"])")</f>
         <v>$DEFINE INST_CALL_INDB_2 (SM_EX2 &amp; opcf:['b'0110110])</v>
       </c>
       <c r="Q66" s="196" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R66" s="211"/>
       <c r="S66" s="78"/>
@@ -14448,7 +14472,7 @@
         <v>58</v>
       </c>
       <c r="T67" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U67" s="212" t="str">
         <f t="shared" si="5"/>
@@ -14563,13 +14587,13 @@
       </c>
       <c r="L68" s="140"/>
       <c r="M68" s="178" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N68" s="140" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="O68" s="140" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="P68" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O68," (SM_EX1 &amp; opcf:['b'",H68,"])")</f>
@@ -14583,14 +14607,14 @@
         <v>58</v>
       </c>
       <c r="T68" s="143" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U68" s="209" t="str">
         <f t="shared" si="5"/>
         <v>11 100</v>
       </c>
       <c r="V68" s="144" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W68" s="145">
         <v>16</v>
@@ -14757,10 +14781,10 @@
       <c r="L69" s="153"/>
       <c r="M69" s="179"/>
       <c r="N69" s="153" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O69" s="153" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="P69" s="15" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O69," (SM_EX2 &amp; opcf:['b'",H69,"])")</f>
@@ -14962,7 +14986,7 @@
         <v>19</v>
       </c>
       <c r="T70" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U70" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15084,7 +15108,7 @@
         <v>19</v>
       </c>
       <c r="T71" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U71" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15206,7 +15230,7 @@
         <v>19</v>
       </c>
       <c r="T72" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U72" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15328,7 +15352,7 @@
         <v>19</v>
       </c>
       <c r="T73" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U73" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15446,7 +15470,7 @@
         <v>19</v>
       </c>
       <c r="T74" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U74" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15564,7 +15588,7 @@
         <v>19</v>
       </c>
       <c r="T75" s="112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U75" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15682,7 +15706,7 @@
         <v>19</v>
       </c>
       <c r="T76" s="114" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U76" s="212" t="str">
         <f t="shared" si="5"/>
@@ -15800,7 +15824,7 @@
         <v>19</v>
       </c>
       <c r="T77" s="81" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U77" s="213" t="str">
         <f t="shared" si="5"/>
@@ -15918,7 +15942,7 @@
         <v>19</v>
       </c>
       <c r="T78" s="83" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U78" s="213" t="str">
         <f t="shared" ref="U78:U143" si="18">_xlfn.CONCAT(MID(DEC2BIN(B78,8),3,2)," ",MID(DEC2BIN(B78,8),5,3))</f>
@@ -16032,16 +16056,16 @@
         <v>24</v>
       </c>
       <c r="L79" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M79" s="24" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="N79" s="115" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O79" s="115" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="P79" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O79," (SM_EX1 &amp; opcf:['b'",H79,"])")</f>
@@ -16051,20 +16075,20 @@
         <v>12</v>
       </c>
       <c r="R79" s="116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S79" s="117" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T79" s="116" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U79" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 001</v>
       </c>
       <c r="V79" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W79" s="68"/>
       <c r="X79" s="68"/>
@@ -16244,16 +16268,16 @@
         <v>24</v>
       </c>
       <c r="L80" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M80" s="24" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="N80" s="115" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="O80" s="115" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="P80" s="21" t="str">
         <f t="shared" ref="P80:P83" si="19">_xlfn.CONCAT("$DEFINE ",O80," (SM_EX1 &amp; opcf:['b'",H80,"])")</f>
@@ -16261,20 +16285,20 @@
       </c>
       <c r="Q80" s="115"/>
       <c r="R80" s="116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S80" s="117" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T80" s="116" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U80" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 001</v>
       </c>
       <c r="V80" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W80" s="68"/>
       <c r="X80" s="68"/>
@@ -16454,16 +16478,16 @@
         <v>24</v>
       </c>
       <c r="L81" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M81" s="24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="N81" s="115" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="O81" s="115" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="P81" s="21" t="str">
         <f t="shared" si="19"/>
@@ -16473,20 +16497,20 @@
         <v>7</v>
       </c>
       <c r="R81" s="116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S81" s="117" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T81" s="116" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U81" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 010</v>
       </c>
       <c r="V81" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W81" s="68"/>
       <c r="X81" s="68"/>
@@ -16666,16 +16690,16 @@
         <v>24</v>
       </c>
       <c r="L82" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M82" s="24" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="N82" s="115" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O82" s="115" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="P82" s="21" t="str">
         <f t="shared" si="19"/>
@@ -16683,20 +16707,20 @@
       </c>
       <c r="Q82" s="115"/>
       <c r="R82" s="116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S82" s="117" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T82" s="116" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U82" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 010</v>
       </c>
       <c r="V82" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W82" s="68"/>
       <c r="X82" s="68"/>
@@ -16876,16 +16900,16 @@
         <v>24</v>
       </c>
       <c r="L83" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M83" s="24" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="N83" s="115" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="O83" s="115" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="P83" s="21" t="str">
         <f t="shared" si="19"/>
@@ -16895,20 +16919,20 @@
         <v>16</v>
       </c>
       <c r="R83" s="116" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S83" s="117" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T83" s="116" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U83" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 011</v>
       </c>
       <c r="V83" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W83" s="68"/>
       <c r="X83" s="68"/>
@@ -17092,7 +17116,7 @@
       <c r="R84" s="116"/>
       <c r="S84" s="117"/>
       <c r="T84" s="116" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U84" s="214" t="str">
         <f t="shared" si="18"/>
@@ -17206,16 +17230,16 @@
         <v>24</v>
       </c>
       <c r="L85" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M85" s="24" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="N85" s="115" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O85" s="115" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="P85" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O85," (SM_EX1 &amp; opcf:['b'",H85,"])")</f>
@@ -17225,20 +17249,20 @@
         <v>15</v>
       </c>
       <c r="R85" s="116" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S85" s="117" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T85" s="116" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U85" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 100</v>
       </c>
       <c r="V85" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W85" s="68"/>
       <c r="X85" s="68"/>
@@ -17422,7 +17446,7 @@
       <c r="R86" s="116"/>
       <c r="S86" s="117"/>
       <c r="T86" s="116" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U86" s="214" t="str">
         <f t="shared" si="18"/>
@@ -17536,16 +17560,16 @@
         <v>24</v>
       </c>
       <c r="L87" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M87" s="24" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="N87" s="115" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="O87" s="115" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="P87" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O87," (SM_EX1 &amp; opcf:['b'",H87,"])")</f>
@@ -17555,20 +17579,20 @@
         <v>14</v>
       </c>
       <c r="R87" s="116" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S87" s="117" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T87" s="116" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U87" s="214" t="str">
         <f t="shared" si="18"/>
         <v>00 101</v>
       </c>
       <c r="V87" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W87" s="68"/>
       <c r="X87" s="68"/>
@@ -17756,7 +17780,7 @@
         <v>19</v>
       </c>
       <c r="T88" s="83" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U88" s="213" t="str">
         <f t="shared" si="18"/>
@@ -17884,7 +17908,7 @@
         <v>19</v>
       </c>
       <c r="T89" s="83" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U89" s="213" t="str">
         <f t="shared" si="18"/>
@@ -18006,7 +18030,7 @@
         <v>19</v>
       </c>
       <c r="T90" s="83" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U90" s="213" t="str">
         <f t="shared" si="18"/>
@@ -18126,7 +18150,7 @@
         <v>19</v>
       </c>
       <c r="T91" s="84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U91" s="213" t="str">
         <f t="shared" si="18"/>
@@ -18244,7 +18268,7 @@
         <v>19</v>
       </c>
       <c r="T92" s="83" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U92" s="213" t="str">
         <f t="shared" si="18"/>
@@ -18358,39 +18382,39 @@
         <v>60</v>
       </c>
       <c r="L93" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M93" s="24" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="N93" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O93" s="21" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="P93" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O93," (SM_EX1 &amp; opcf:['b'",H93,"])")</f>
         <v>$DEFINE INST_STOREW_A_INDI16 (SM_EX1 &amp; opcf:['b'1010000])</v>
       </c>
       <c r="Q93" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R93" s="83" t="s">
         <v>58</v>
       </c>
       <c r="S93" s="80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T93" s="81" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U93" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 000</v>
       </c>
       <c r="V93" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W93" s="68">
         <v>16</v>
@@ -18572,39 +18596,39 @@
         <v>60</v>
       </c>
       <c r="L94" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M94" s="24" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="N94" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O94" s="21" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P94" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O94," (SM_EX1 &amp; opcf:['b'",H94,"])")</f>
         <v>$DEFINE INST_STOREB_A_INDI16 (SM_EX1 &amp; opcf:['b'1010001])</v>
       </c>
       <c r="Q94" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R94" s="83" t="s">
         <v>58</v>
       </c>
       <c r="S94" s="82" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="T94" s="83" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U94" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 000</v>
       </c>
       <c r="V94" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W94" s="68">
         <v>8</v>
@@ -18683,13 +18707,13 @@
         <v>1</v>
       </c>
       <c r="AY94" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ94" s="104">
         <v>0</v>
       </c>
       <c r="BA94" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB94" s="104">
         <v>0</v>
@@ -18703,10 +18727,10 @@
         <v>0</v>
       </c>
       <c r="BG94" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH94" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI94" s="60"/>
       <c r="BJ94" s="106">
@@ -18783,22 +18807,22 @@
       <c r="K95" s="24"/>
       <c r="L95" s="21"/>
       <c r="M95" s="272" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="N95" s="273" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="O95" s="21"/>
       <c r="P95" s="21"/>
       <c r="Q95" s="273" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="R95" s="83"/>
       <c r="S95" s="82" t="s">
         <v>19</v>
       </c>
       <c r="T95" s="83" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U95" s="213" t="str">
         <f t="shared" si="18"/>
@@ -18923,7 +18947,7 @@
         <v>19</v>
       </c>
       <c r="T96" s="83" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U96" s="213" t="str">
         <f t="shared" si="18"/>
@@ -19042,37 +19066,37 @@
         <v>24</v>
       </c>
       <c r="L97" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M97" s="24" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="N97" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O97" s="21" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="P97" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O97," (SM_EX1 &amp; opcf:['b'",H97,"])")</f>
         <v>$DEFINE INST_LOADW_INDI16_C (SM_EX1 &amp; opcf:['b'1010100])</v>
       </c>
       <c r="Q97" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R97" s="83" t="s">
         <v>58</v>
       </c>
       <c r="S97" s="82"/>
       <c r="T97" s="83" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U97" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 010</v>
       </c>
       <c r="V97" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W97" s="68">
         <v>16</v>
@@ -19254,37 +19278,37 @@
         <v>24</v>
       </c>
       <c r="L98" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M98" s="24" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="N98" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O98" s="21" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P98" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O98," (SM_EX1 &amp; opcf:['b'",H98,"])")</f>
         <v>$DEFINE INST_LOADB_INDI16_C (SM_EX1 &amp; opcf:['b'1010101])</v>
       </c>
       <c r="Q98" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R98" s="83" t="s">
         <v>58</v>
       </c>
       <c r="S98" s="82"/>
       <c r="T98" s="83" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U98" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 010</v>
       </c>
       <c r="V98" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W98" s="68">
         <v>8</v>
@@ -19363,13 +19387,13 @@
         <v>1</v>
       </c>
       <c r="AY98" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ98" s="62" t="s">
         <v>58</v>
       </c>
       <c r="BA98" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB98" s="106">
         <v>1</v>
@@ -19383,10 +19407,10 @@
         <v>0</v>
       </c>
       <c r="BG98" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH98" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI98" s="60"/>
       <c r="BJ98" s="106">
@@ -19472,14 +19496,14 @@
         <v>58</v>
       </c>
       <c r="T99" s="83" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U99" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 011</v>
       </c>
       <c r="V99" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W99" s="68"/>
       <c r="X99" s="68"/>
@@ -19591,7 +19615,7 @@
       <c r="R100" s="83"/>
       <c r="S100" s="82"/>
       <c r="T100" s="83" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U100" s="213" t="str">
         <f t="shared" si="18"/>
@@ -19705,23 +19729,23 @@
         <v>24</v>
       </c>
       <c r="L101" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M101" s="24" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N101" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O101" s="21" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="P101" s="21" t="str">
         <f t="shared" ref="P101:P107" si="20">_xlfn.CONCAT("$DEFINE ",O101," (SM_EX1 &amp; opcf:['b'",H101,"])")</f>
         <v>$DEFINE INST_JMP_I16 (SM_EX1 &amp; opcf:['b'1011000])</v>
       </c>
       <c r="Q101" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R101" s="83" t="s">
         <v>58</v>
@@ -19730,14 +19754,14 @@
         <v>58</v>
       </c>
       <c r="T101" s="83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U101" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 100</v>
       </c>
       <c r="V101" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W101" s="68"/>
       <c r="X101" s="70" t="s">
@@ -19919,23 +19943,23 @@
         <v>24</v>
       </c>
       <c r="L102" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M102" s="24" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="N102" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O102" s="21" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="P102" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JZ_I16 (SM_EX1 &amp; opcf:['b'1011001])</v>
       </c>
       <c r="Q102" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R102" s="83" t="s">
         <v>58</v>
@@ -19944,14 +19968,14 @@
         <v>58</v>
       </c>
       <c r="T102" s="83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U102" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 100</v>
       </c>
       <c r="V102" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W102" s="68"/>
       <c r="X102" s="70" t="s">
@@ -20133,23 +20157,23 @@
         <v>24</v>
       </c>
       <c r="L103" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M103" s="24" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="N103" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O103" s="21" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="P103" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JNZ_I16 (SM_EX1 &amp; opcf:['b'1011010])</v>
       </c>
       <c r="Q103" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R103" s="83" t="s">
         <v>58</v>
@@ -20158,14 +20182,14 @@
         <v>58</v>
       </c>
       <c r="T103" s="83" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U103" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 101</v>
       </c>
       <c r="V103" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W103" s="68"/>
       <c r="X103" s="70" t="s">
@@ -20347,23 +20371,23 @@
         <v>24</v>
       </c>
       <c r="L104" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M104" s="24" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="N104" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O104" s="21" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P104" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JC_I16 (SM_EX1 &amp; opcf:['b'1011011])</v>
       </c>
       <c r="Q104" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R104" s="83" t="s">
         <v>58</v>
@@ -20372,14 +20396,14 @@
         <v>58</v>
       </c>
       <c r="T104" s="83" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U104" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 101</v>
       </c>
       <c r="V104" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W104" s="68"/>
       <c r="X104" s="70" t="s">
@@ -20561,23 +20585,23 @@
         <v>24</v>
       </c>
       <c r="L105" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M105" s="24" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="N105" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O105" s="21" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P105" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JNC_I16 (SM_EX1 &amp; opcf:['b'1011100])</v>
       </c>
       <c r="Q105" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R105" s="83" t="s">
         <v>58</v>
@@ -20586,14 +20610,14 @@
         <v>58</v>
       </c>
       <c r="T105" s="83" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U105" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 110</v>
       </c>
       <c r="V105" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W105" s="68"/>
       <c r="X105" s="70" t="s">
@@ -20775,23 +20799,23 @@
         <v>24</v>
       </c>
       <c r="L106" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M106" s="24" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="N106" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O106" s="21" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="P106" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JV_I16 (SM_EX1 &amp; opcf:['b'1011101])</v>
       </c>
       <c r="Q106" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R106" s="83" t="s">
         <v>58</v>
@@ -20800,14 +20824,14 @@
         <v>58</v>
       </c>
       <c r="T106" s="83" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U106" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 110</v>
       </c>
       <c r="V106" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W106" s="68"/>
       <c r="X106" s="70" t="s">
@@ -20989,23 +21013,23 @@
         <v>24</v>
       </c>
       <c r="L107" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M107" s="24" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="N107" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O107" s="21" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="P107" s="21" t="str">
         <f t="shared" si="20"/>
         <v>$DEFINE INST_JNV_I16 (SM_EX1 &amp; opcf:['b'1011110])</v>
       </c>
       <c r="Q107" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R107" s="83" t="s">
         <v>58</v>
@@ -21014,14 +21038,14 @@
         <v>58</v>
       </c>
       <c r="T107" s="84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U107" s="213" t="str">
         <f t="shared" si="18"/>
         <v>01 111</v>
       </c>
       <c r="V107" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W107" s="68"/>
       <c r="X107" s="70" t="s">
@@ -21197,11 +21221,11 @@
       <c r="J108" s="24"/>
       <c r="K108" s="24"/>
       <c r="L108" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M108" s="24"/>
       <c r="N108" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="O108" s="21"/>
       <c r="P108" s="21"/>
@@ -21213,7 +21237,7 @@
         <v>19</v>
       </c>
       <c r="T108" s="83" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U108" s="213" t="str">
         <f t="shared" si="18"/>
@@ -21330,23 +21354,23 @@
         <v>60</v>
       </c>
       <c r="L109" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M109" s="24" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="N109" s="21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O109" s="21" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="P109" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O109," (SM_EX1 &amp; opcf:['b'",H109,"])")</f>
         <v>$DEFINE INST_STOREW_A_RI16 (SM_EX1 &amp; opcf:['b'1100000])</v>
       </c>
       <c r="Q109" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="R109" s="83" t="s">
         <v>58</v>
@@ -21355,14 +21379,14 @@
         <v>58</v>
       </c>
       <c r="T109" s="86" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U109" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 000</v>
       </c>
       <c r="V109" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W109" s="68">
         <v>16</v>
@@ -21544,23 +21568,23 @@
         <v>60</v>
       </c>
       <c r="L110" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M110" s="24" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="N110" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O110" s="21" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="P110" s="21" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O110," (SM_EX1 &amp; opcf:['b'",H110,"])")</f>
         <v>$DEFINE INST_STOREB_A_RI16 (SM_EX1 &amp; opcf:['b'1100001])</v>
       </c>
       <c r="Q110" s="21" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="R110" s="83" t="s">
         <v>58</v>
@@ -21569,14 +21593,14 @@
         <v>58</v>
       </c>
       <c r="T110" s="87" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U110" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 000</v>
       </c>
       <c r="V110" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W110" s="68">
         <v>8</v>
@@ -21655,13 +21679,13 @@
         <v>1</v>
       </c>
       <c r="AY110" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ110" s="104">
         <v>0</v>
       </c>
       <c r="BA110" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB110" s="104">
         <v>0</v>
@@ -21675,10 +21699,10 @@
         <v>0</v>
       </c>
       <c r="BG110" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH110" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI110" s="60"/>
       <c r="BJ110" s="106">
@@ -21762,7 +21786,7 @@
         <v>19</v>
       </c>
       <c r="T111" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U111" s="213" t="str">
         <f t="shared" si="18"/>
@@ -21880,7 +21904,7 @@
         <v>19</v>
       </c>
       <c r="T112" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U112" s="213" t="str">
         <f t="shared" si="18"/>
@@ -21994,23 +22018,23 @@
         <v>24</v>
       </c>
       <c r="L113" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M113" s="24" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="N113" s="21" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="O113" s="21" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="P113" s="21" t="str">
         <f t="shared" ref="P113:P115" si="21">_xlfn.CONCAT("$DEFINE ",O113," (SM_EX1 &amp; opcf:['b'",H113,"])")</f>
         <v>$DEFINE INST_LOADW_RI16_C (SM_EX1 &amp; opcf:['b'1100100])</v>
       </c>
       <c r="Q113" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="R113" s="83" t="s">
         <v>58</v>
@@ -22019,14 +22043,14 @@
         <v>58</v>
       </c>
       <c r="T113" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U113" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 010</v>
       </c>
       <c r="V113" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W113" s="68">
         <v>16</v>
@@ -22208,23 +22232,23 @@
         <v>24</v>
       </c>
       <c r="L114" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M114" s="24" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="N114" s="21" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O114" s="21" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="P114" s="21" t="str">
         <f t="shared" si="21"/>
         <v>$DEFINE INST_LOADB_RI16_C (SM_EX1 &amp; opcf:['b'1100101])</v>
       </c>
       <c r="Q114" s="21" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="R114" s="83" t="s">
         <v>58</v>
@@ -22233,14 +22257,14 @@
         <v>58</v>
       </c>
       <c r="T114" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U114" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 010</v>
       </c>
       <c r="V114" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W114" s="68">
         <v>8</v>
@@ -22319,13 +22343,13 @@
         <v>1</v>
       </c>
       <c r="AY114" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AZ114" s="62" t="s">
         <v>58</v>
       </c>
       <c r="BA114" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BB114" s="106">
         <v>1</v>
@@ -22339,10 +22363,10 @@
         <v>0</v>
       </c>
       <c r="BG114" s="70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH114" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BI114" s="60"/>
       <c r="BJ114" s="106">
@@ -22422,16 +22446,16 @@
         <v>24</v>
       </c>
       <c r="L115" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M115" s="24" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="N115" s="21" t="s">
         <v>68</v>
       </c>
       <c r="O115" s="21" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="P115" s="21" t="str">
         <f t="shared" si="21"/>
@@ -22447,14 +22471,14 @@
         <v>58</v>
       </c>
       <c r="T115" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U115" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 011</v>
       </c>
       <c r="V115" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W115" s="68"/>
       <c r="X115" s="68"/>
@@ -22638,7 +22662,7 @@
         <v>58</v>
       </c>
       <c r="T116" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U116" s="213" t="str">
         <f t="shared" si="18"/>
@@ -22748,23 +22772,23 @@
         <v>24</v>
       </c>
       <c r="L117" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M117" s="24" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="N117" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O117" s="21" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="P117" s="21" t="str">
         <f t="shared" ref="P117:P123" si="22">_xlfn.CONCAT("$DEFINE ",O117," (SM_EX1 &amp; opcf:['b'",H117,"])")</f>
         <v>$DEFINE INST_JMP_INDI16 (SM_EX1 &amp; opcf:['b'1101000])</v>
       </c>
       <c r="Q117" s="21" t="s">
-        <v>137</v>
+        <v>419</v>
       </c>
       <c r="R117" s="83" t="s">
         <v>58</v>
@@ -22773,14 +22797,14 @@
         <v>58</v>
       </c>
       <c r="T117" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U117" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 100</v>
       </c>
       <c r="V117" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W117" s="68"/>
       <c r="X117" s="70" t="s">
@@ -22958,23 +22982,23 @@
         <v>24</v>
       </c>
       <c r="L118" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M118" s="24" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="N118" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O118" s="21" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="P118" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JZ_INDI16 (SM_EX1 &amp; opcf:['b'1101001])</v>
       </c>
       <c r="Q118" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="R118" s="83" t="s">
         <v>58</v>
@@ -22983,14 +23007,14 @@
         <v>58</v>
       </c>
       <c r="T118" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U118" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 100</v>
       </c>
       <c r="V118" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W118" s="68"/>
       <c r="X118" s="70" t="s">
@@ -23168,23 +23192,23 @@
         <v>24</v>
       </c>
       <c r="L119" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M119" s="24" t="s">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="N119" s="21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O119" s="21" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="P119" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JNZ_INDI16 (SM_EX1 &amp; opcf:['b'1101010])</v>
       </c>
       <c r="Q119" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="R119" s="83" t="s">
         <v>58</v>
@@ -23193,14 +23217,14 @@
         <v>58</v>
       </c>
       <c r="T119" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U119" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 101</v>
       </c>
       <c r="V119" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W119" s="68"/>
       <c r="X119" s="70" t="s">
@@ -23378,23 +23402,23 @@
         <v>24</v>
       </c>
       <c r="L120" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M120" s="24" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="N120" s="21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O120" s="21" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="P120" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JC_INDI16 (SM_EX1 &amp; opcf:['b'1101011])</v>
       </c>
       <c r="Q120" s="21" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="R120" s="83" t="s">
         <v>58</v>
@@ -23403,14 +23427,14 @@
         <v>58</v>
       </c>
       <c r="T120" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U120" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 101</v>
       </c>
       <c r="V120" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W120" s="68"/>
       <c r="X120" s="70" t="s">
@@ -23588,23 +23612,23 @@
         <v>24</v>
       </c>
       <c r="L121" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M121" s="24" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="N121" s="21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="O121" s="21" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="P121" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JNC_INDI16 (SM_EX1 &amp; opcf:['b'1101100])</v>
       </c>
       <c r="Q121" s="21" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R121" s="83" t="s">
         <v>58</v>
@@ -23613,14 +23637,14 @@
         <v>58</v>
       </c>
       <c r="T121" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U121" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 110</v>
       </c>
       <c r="V121" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W121" s="68"/>
       <c r="X121" s="70" t="s">
@@ -23798,23 +23822,23 @@
         <v>24</v>
       </c>
       <c r="L122" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M122" s="24" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="N122" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="O122" s="21" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="P122" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JV_INDI16 (SM_EX1 &amp; opcf:['b'1101101])</v>
       </c>
       <c r="Q122" s="21" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="R122" s="83" t="s">
         <v>58</v>
@@ -23823,14 +23847,14 @@
         <v>58</v>
       </c>
       <c r="T122" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U122" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 110</v>
       </c>
       <c r="V122" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W122" s="68"/>
       <c r="X122" s="70" t="s">
@@ -24008,23 +24032,23 @@
         <v>24</v>
       </c>
       <c r="L123" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M123" s="24" t="s">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="N123" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O123" s="21" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="P123" s="21" t="str">
         <f t="shared" si="22"/>
         <v>$DEFINE INST_JNV_INDI16 (SM_EX1 &amp; opcf:['b'1101110])</v>
       </c>
       <c r="Q123" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="R123" s="83" t="s">
         <v>58</v>
@@ -24033,14 +24057,14 @@
         <v>58</v>
       </c>
       <c r="T123" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U123" s="213" t="str">
         <f t="shared" si="18"/>
         <v>10 111</v>
       </c>
       <c r="V123" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W123" s="68"/>
       <c r="X123" s="70" t="s">
@@ -24216,11 +24240,11 @@
       <c r="J124" s="24"/>
       <c r="K124" s="24"/>
       <c r="L124" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M124" s="24"/>
       <c r="N124" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="O124" s="21"/>
       <c r="P124" s="21"/>
@@ -24232,7 +24256,7 @@
         <v>58</v>
       </c>
       <c r="T124" s="88" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U124" s="213" t="str">
         <f t="shared" si="18"/>
@@ -24353,7 +24377,7 @@
         <v>19</v>
       </c>
       <c r="T125" s="90" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U125" s="216" t="str">
         <f t="shared" si="18"/>
@@ -24471,7 +24495,7 @@
         <v>19</v>
       </c>
       <c r="T126" s="92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="U126" s="216" t="str">
         <f t="shared" si="18"/>
@@ -24589,7 +24613,7 @@
         <v>19</v>
       </c>
       <c r="T127" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U127" s="216" t="str">
         <f t="shared" si="18"/>
@@ -24707,7 +24731,7 @@
         <v>19</v>
       </c>
       <c r="T128" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U128" s="216" t="str">
         <f t="shared" si="18"/>
@@ -24825,7 +24849,7 @@
         <v>19</v>
       </c>
       <c r="T129" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U129" s="216" t="str">
         <f t="shared" ref="U129" si="23">_xlfn.CONCAT(MID(DEC2BIN(B129,8),3,2)," ",MID(DEC2BIN(B129,8),5,3))</f>
@@ -24932,7 +24956,7 @@
         <v>19</v>
       </c>
       <c r="T130" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U130" s="216" t="str">
         <f t="shared" si="18"/>
@@ -25050,7 +25074,7 @@
         <v>19</v>
       </c>
       <c r="T131" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U131" s="216" t="str">
         <f t="shared" si="18"/>
@@ -25165,28 +25189,28 @@
         <v>24</v>
       </c>
       <c r="L132" s="195" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M132" s="66"/>
       <c r="N132" s="195" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O132" s="195" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="P132" s="195" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O132," (SM_EX1 &amp; opcf:['b'",H132,"])")</f>
         <v>$DEFINE INST_CALL_INDI16 (SM_EX1 &amp; opcf:['b'1110110])</v>
       </c>
       <c r="Q132" s="195" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R132" s="215"/>
       <c r="S132" s="91" t="s">
         <v>58</v>
       </c>
       <c r="T132" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U132" s="216" t="str">
         <f t="shared" si="18"/>
@@ -25306,7 +25330,7 @@
         <v>58</v>
       </c>
       <c r="T133" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U133" s="216" t="str">
         <f t="shared" si="18"/>
@@ -25416,16 +25440,16 @@
         <v>24</v>
       </c>
       <c r="L134" s="197" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M134" s="266" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="N134" s="267" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O134" s="197" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="P134" s="195" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O134," (SM_EX1 &amp; opcf:['b'",H134,"])")</f>
@@ -25439,14 +25463,14 @@
         <v>58</v>
       </c>
       <c r="T134" s="174" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U134" s="217" t="str">
         <f t="shared" si="18"/>
         <v>11 100</v>
       </c>
       <c r="V134" s="144" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W134" s="145">
         <v>16</v>
@@ -25613,14 +25637,14 @@
         <v>24</v>
       </c>
       <c r="L135" s="198" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M135" s="181"/>
       <c r="N135" s="198" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="O135" s="197" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="P135" s="195" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O135," (SM_EX2 &amp; opcf:['b'",H135,"])")</f>
@@ -25814,16 +25838,16 @@
         <v>24</v>
       </c>
       <c r="L136" s="197" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M136" s="266" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="N136" s="267" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O136" s="197" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="P136" s="195" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O136," (SM_EX1 &amp; opcf:['b'",H136,"])")</f>
@@ -25837,14 +25861,14 @@
         <v>58</v>
       </c>
       <c r="T136" s="174" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U136" s="217" t="str">
         <f t="shared" si="18"/>
         <v>11 100</v>
       </c>
       <c r="V136" s="144" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W136" s="145">
         <v>16</v>
@@ -26011,14 +26035,14 @@
         <v>24</v>
       </c>
       <c r="L137" s="198" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M137" s="181"/>
       <c r="N137" s="198" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O137" s="197" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="P137" s="195" t="str">
         <f>_xlfn.CONCAT("$DEFINE ",O137," (SM_EX2 &amp; opcf:['b'",H137,"])")</f>
@@ -26214,7 +26238,7 @@
       <c r="R138" s="215"/>
       <c r="S138" s="91"/>
       <c r="T138" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U138" s="216" t="str">
         <f t="shared" si="18"/>
@@ -26330,7 +26354,7 @@
       <c r="R139" s="215"/>
       <c r="S139" s="91"/>
       <c r="T139" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U139" s="216" t="str">
         <f t="shared" si="18"/>
@@ -26446,7 +26470,7 @@
       <c r="R140" s="215"/>
       <c r="S140" s="91"/>
       <c r="T140" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U140" s="216" t="str">
         <f t="shared" si="18"/>
@@ -26562,7 +26586,7 @@
       <c r="R141" s="215"/>
       <c r="S141" s="91"/>
       <c r="T141" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U141" s="216" t="str">
         <f t="shared" si="18"/>
@@ -26678,7 +26702,7 @@
       <c r="R142" s="215"/>
       <c r="S142" s="91"/>
       <c r="T142" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U142" s="216" t="str">
         <f t="shared" si="18"/>
@@ -26796,14 +26820,14 @@
       <c r="R143" s="224"/>
       <c r="S143" s="225"/>
       <c r="T143" s="226" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="U143" s="227" t="str">
         <f t="shared" si="18"/>
         <v>11 111</v>
       </c>
       <c r="V143" s="95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W143" s="68"/>
       <c r="X143" s="68"/>
@@ -26996,16 +27020,16 @@
       <c r="B3" s="185"/>
       <c r="C3" s="185"/>
       <c r="D3" s="55" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E3" s="185" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F3" s="55" t="s">
         <v>63</v>
       </c>
       <c r="K3" s="243" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="17" thickBot="1">
@@ -27027,11 +27051,11 @@
         <v>0</v>
       </c>
       <c r="S4" s="251" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="T4" s="251"/>
       <c r="U4" s="251" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="V4" s="251"/>
     </row>
@@ -27044,7 +27068,7 @@
         <v>#1</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E5" s="189">
         <v>1</v>
@@ -27054,7 +27078,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="237" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="L5" s="238" t="s">
         <v>34</v>
@@ -27066,28 +27090,28 @@
         <v>59</v>
       </c>
       <c r="O5" s="238" t="s">
+        <v>394</v>
+      </c>
+      <c r="P5" s="239" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q5" s="238" t="s">
+        <v>402</v>
+      </c>
+      <c r="R5" s="238" t="s">
+        <v>404</v>
+      </c>
+      <c r="S5" s="239" t="s">
+        <v>399</v>
+      </c>
+      <c r="T5" s="239" t="s">
         <v>398</v>
       </c>
-      <c r="P5" s="239" t="s">
+      <c r="U5" s="239" t="s">
         <v>399</v>
       </c>
-      <c r="Q5" s="238" t="s">
-        <v>406</v>
-      </c>
-      <c r="R5" s="238" t="s">
-        <v>408</v>
-      </c>
-      <c r="S5" s="239" t="s">
-        <v>403</v>
-      </c>
-      <c r="T5" s="239" t="s">
-        <v>402</v>
-      </c>
-      <c r="U5" s="239" t="s">
-        <v>403</v>
-      </c>
       <c r="V5" s="240" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="17" thickBot="1">
@@ -27099,7 +27123,7 @@
         <v>#2</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E6" s="189">
         <v>2</v>
@@ -27109,7 +27133,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="L6" s="235">
         <v>5</v>
@@ -27161,7 +27185,7 @@
         <v>#3</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E7" s="189">
         <v>3</v>
@@ -27171,7 +27195,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="L7" s="235">
         <v>1</v>
@@ -27223,7 +27247,7 @@
         <v>#4</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E8" s="189">
         <v>4</v>
@@ -27233,7 +27257,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="L8" s="235">
         <v>2</v>
@@ -27285,7 +27309,7 @@
         <v>#5</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E9" s="189">
         <v>5</v>
@@ -27295,7 +27319,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="L9" s="235">
         <v>1</v>
@@ -27357,7 +27381,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="L10" s="235">
         <v>4</v>
@@ -27638,7 +27662,7 @@
         <v>#C</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E16" s="189">
         <v>12</v>
@@ -27820,7 +27844,7 @@
         <v>#10</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E20" s="189">
         <v>16</v>
@@ -27867,7 +27891,7 @@
         <v>#11</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E21" s="189">
         <v>17</v>
@@ -27914,7 +27938,7 @@
         <v>#12</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E22" s="189">
         <v>18</v>
@@ -27961,7 +27985,7 @@
         <v>#13</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E23" s="189">
         <v>19</v>
@@ -28008,7 +28032,7 @@
         <v>#14</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E24" s="189">
         <v>20</v>
@@ -28055,7 +28079,7 @@
         <v>#15</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E25" s="189">
         <v>21</v>
@@ -28192,7 +28216,7 @@
         <v>#18</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E28" s="189">
         <v>24</v>
@@ -28239,7 +28263,7 @@
         <v>#19</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E29" s="189">
         <v>25</v>
@@ -28286,7 +28310,7 @@
         <v>#1A</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E30" s="189">
         <v>26</v>
@@ -28333,7 +28357,7 @@
         <v>#1B</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E31" s="189">
         <v>27</v>
@@ -28380,7 +28404,7 @@
         <v>#1C</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E32" s="189">
         <v>28</v>
@@ -28427,7 +28451,7 @@
         <v>#1D</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E33" s="189">
         <v>29</v>
@@ -28474,7 +28498,7 @@
         <v>#1E</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E34" s="189">
         <v>30</v>
@@ -28656,7 +28680,7 @@
         <v>#22</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E38" s="189">
         <v>34</v>
@@ -28703,7 +28727,7 @@
         <v>#23</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E39" s="189">
         <v>35</v>
@@ -28750,7 +28774,7 @@
         <v>#24</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E40" s="189">
         <v>36</v>
@@ -28797,7 +28821,7 @@
         <v>#25</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E41" s="189">
         <v>37</v>
@@ -29024,7 +29048,7 @@
         <v>#2A</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E46" s="189">
         <v>42</v>
@@ -29071,7 +29095,7 @@
         <v>#2B</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E47" s="189">
         <v>43</v>
@@ -29118,7 +29142,7 @@
         <v>#2C</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E48" s="189">
         <v>44</v>
@@ -29165,7 +29189,7 @@
         <v>#2D</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E49" s="189">
         <v>45</v>
@@ -29184,7 +29208,7 @@
         <v>#2E</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E50" s="189">
         <v>46</v>
@@ -29220,7 +29244,7 @@
         <v>#30</v>
       </c>
       <c r="D52" s="178" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E52" s="189">
         <v>48</v>
@@ -29303,7 +29327,7 @@
         <v>#34</v>
       </c>
       <c r="D57" s="178" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E57" s="189">
         <v>52</v>
@@ -29399,7 +29423,7 @@
         <v>#38</v>
       </c>
       <c r="D63" s="178" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E63" s="189">
         <v>56</v>
@@ -29584,7 +29608,7 @@
         <v>#42</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E74" s="189">
         <v>66</v>
@@ -29603,7 +29627,7 @@
         <v>#43</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E75" s="189">
         <v>67</v>
@@ -29622,7 +29646,7 @@
         <v>#44</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E76" s="189">
         <v>68</v>
@@ -29641,7 +29665,7 @@
         <v>#45</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E77" s="189">
         <v>69</v>
@@ -29660,7 +29684,7 @@
         <v>#46</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E78" s="189">
         <v>70</v>
@@ -29696,7 +29720,7 @@
         <v>#48</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E80" s="189">
         <v>72</v>
@@ -29732,7 +29756,7 @@
         <v>#4A</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E82" s="189">
         <v>74</v>
@@ -29836,7 +29860,7 @@
         <v>#50</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E88" s="189">
         <v>80</v>
@@ -29855,7 +29879,7 @@
         <v>#51</v>
       </c>
       <c r="D89" s="24" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E89" s="189">
         <v>81</v>
@@ -29908,7 +29932,7 @@
         <v>#54</v>
       </c>
       <c r="D92" s="24" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E92" s="189">
         <v>84</v>
@@ -29927,7 +29951,7 @@
         <v>#55</v>
       </c>
       <c r="D93" s="24" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E93" s="189">
         <v>85</v>
@@ -29980,7 +30004,7 @@
         <v>#58</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E96" s="189">
         <v>88</v>
@@ -29999,7 +30023,7 @@
         <v>#59</v>
       </c>
       <c r="D97" s="24" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E97" s="189">
         <v>89</v>
@@ -30018,7 +30042,7 @@
         <v>#5A</v>
       </c>
       <c r="D98" s="24" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E98" s="189">
         <v>90</v>
@@ -30037,7 +30061,7 @@
         <v>#5B</v>
       </c>
       <c r="D99" s="24" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E99" s="189">
         <v>91</v>
@@ -30056,7 +30080,7 @@
         <v>#5C</v>
       </c>
       <c r="D100" s="24" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E100" s="189">
         <v>92</v>
@@ -30075,7 +30099,7 @@
         <v>#5D</v>
       </c>
       <c r="D101" s="24" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E101" s="189">
         <v>93</v>
@@ -30094,7 +30118,7 @@
         <v>#5E</v>
       </c>
       <c r="D102" s="24" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E102" s="189">
         <v>94</v>
@@ -30130,7 +30154,7 @@
         <v>#60</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E104" s="189">
         <v>96</v>
@@ -30149,7 +30173,7 @@
         <v>#61</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E105" s="189">
         <v>97</v>
@@ -30202,7 +30226,7 @@
         <v>#64</v>
       </c>
       <c r="D108" s="24" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E108" s="189">
         <v>100</v>
@@ -30221,7 +30245,7 @@
         <v>#65</v>
       </c>
       <c r="D109" s="24" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E109" s="189">
         <v>101</v>
@@ -30240,7 +30264,7 @@
         <v>#66</v>
       </c>
       <c r="D110" s="24" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E110" s="189">
         <v>102</v>
@@ -30276,7 +30300,7 @@
         <v>#68</v>
       </c>
       <c r="D112" s="24" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E112" s="189">
         <v>104</v>
@@ -30295,7 +30319,7 @@
         <v>#69</v>
       </c>
       <c r="D113" s="24" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E113" s="189">
         <v>105</v>
@@ -30314,7 +30338,7 @@
         <v>#6A</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E114" s="189">
         <v>106</v>
@@ -30333,7 +30357,7 @@
         <v>#6B</v>
       </c>
       <c r="D115" s="24" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E115" s="189">
         <v>107</v>
@@ -30352,7 +30376,7 @@
         <v>#6C</v>
       </c>
       <c r="D116" s="24" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E116" s="189">
         <v>108</v>
@@ -30371,7 +30395,7 @@
         <v>#6D</v>
       </c>
       <c r="D117" s="24" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E117" s="189">
         <v>109</v>
@@ -30390,7 +30414,7 @@
         <v>#6E</v>
       </c>
       <c r="D118" s="24" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E118" s="189">
         <v>110</v>
@@ -30575,7 +30599,7 @@
         <v>#78</v>
       </c>
       <c r="D129" s="180" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E129" s="189">
         <v>120</v>
@@ -30607,7 +30631,7 @@
         <v>#79</v>
       </c>
       <c r="D131" s="180" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E131" s="189">
         <v>121</v>

</xml_diff>

<commit_message>
Support for EffAdd A2D Routing in SP
</commit_message>
<xml_diff>
--- a/MicroCPUInstructionWord.xlsx
+++ b/MicroCPUInstructionWord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbs/src/Kartana9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B423E75B-D406-1D4C-8E2E-603944136FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D9C4F1-0754-F945-855F-70E390420304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1000" windowWidth="33640" windowHeight="21580" xr2:uid="{1A9992FB-C001-7647-8C04-DC19BDE12C33}"/>
+    <workbookView xWindow="5380" yWindow="760" windowWidth="33640" windowHeight="21580" xr2:uid="{1A9992FB-C001-7647-8C04-DC19BDE12C33}"/>
   </bookViews>
   <sheets>
     <sheet name="MainInstructionCard" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="428">
   <si>
     <t>Instruction Word</t>
   </si>
@@ -1308,6 +1308,24 @@
   </si>
   <si>
     <t>/SP_D2B_OE</t>
+  </si>
+  <si>
+    <t>TESTI</t>
+  </si>
+  <si>
+    <t>TESTI a,imm16</t>
+  </si>
+  <si>
+    <t>Logical AND of Reg-a and imm16, no store</t>
+  </si>
+  <si>
+    <t>SHRC b,cnt,c</t>
+  </si>
+  <si>
+    <t>c = b &gt;&gt; (cnt+1) (carry flag fill)</t>
+  </si>
+  <si>
+    <t>??SHRC??</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2877,6 +2895,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3201,10 +3223,10 @@
   </sheetPr>
   <dimension ref="B1:CN144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2640" topLeftCell="A10" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2640" topLeftCell="A21" activePane="bottomLeft"/>
       <selection activeCell="AH4" sqref="AH4"/>
-      <selection pane="bottomLeft" activeCell="AN27" sqref="AN27"/>
+      <selection pane="bottomLeft" activeCell="AJ88" sqref="AJ88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11349,14 +11371,20 @@
       <c r="J47" s="36"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="75"/>
+      <c r="M47" s="275" t="s">
+        <v>427</v>
+      </c>
+      <c r="N47" s="274" t="s">
+        <v>425</v>
+      </c>
+      <c r="O47" s="274"/>
+      <c r="P47" s="274"/>
+      <c r="Q47" s="274" t="s">
+        <v>426</v>
+      </c>
+      <c r="R47" s="75" t="s">
+        <v>250</v>
+      </c>
       <c r="S47" s="74" t="s">
         <v>58</v>
       </c>
@@ -11370,47 +11398,117 @@
       <c r="W47" s="68"/>
       <c r="X47" s="68"/>
       <c r="Y47" s="60"/>
-      <c r="Z47" s="60"/>
-      <c r="AA47" s="60"/>
-      <c r="AB47" s="60"/>
-      <c r="AC47" s="60"/>
-      <c r="AD47" s="60"/>
-      <c r="AE47" s="60"/>
-      <c r="AF47" s="60"/>
-      <c r="AG47" s="60"/>
-      <c r="AH47" s="60"/>
-      <c r="AI47" s="60"/>
-      <c r="AJ47" s="60"/>
-      <c r="AK47" s="60"/>
-      <c r="AL47" s="60"/>
-      <c r="AM47" s="60"/>
-      <c r="AN47" s="60"/>
-      <c r="AO47" s="60"/>
-      <c r="AP47" s="60"/>
-      <c r="AQ47" s="60"/>
-      <c r="AR47" s="60"/>
-      <c r="AS47" s="60"/>
-      <c r="AT47" s="60"/>
-      <c r="AU47" s="60"/>
-      <c r="AV47" s="60"/>
+      <c r="Z47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AC47" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD47" s="107">
+        <v>1</v>
+      </c>
+      <c r="AE47" s="107">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="107">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="102" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH47" s="102"/>
+      <c r="AI47" s="107">
+        <v>1</v>
+      </c>
+      <c r="AJ47" s="104">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="107">
+        <v>1</v>
+      </c>
+      <c r="AL47" s="104">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AO47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AQ47" s="104">
+        <v>0</v>
+      </c>
+      <c r="AR47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AS47" s="104">
+        <v>0</v>
+      </c>
+      <c r="AT47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AU47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AV47" s="104">
+        <v>0</v>
+      </c>
       <c r="AW47" s="60"/>
       <c r="AX47" s="60"/>
-      <c r="AY47" s="60"/>
-      <c r="AZ47" s="60"/>
-      <c r="BA47" s="60"/>
-      <c r="BB47" s="60"/>
-      <c r="BC47" s="60"/>
+      <c r="AY47" s="106">
+        <v>1</v>
+      </c>
+      <c r="AZ47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BA47" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BC47" s="62" t="s">
+        <v>58</v>
+      </c>
       <c r="BD47" s="60"/>
       <c r="BE47" s="60"/>
-      <c r="BF47" s="60"/>
-      <c r="BG47" s="60"/>
-      <c r="BH47" s="60"/>
-      <c r="BI47" s="60"/>
+      <c r="BF47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BG47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BH47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BI47" s="106">
+        <v>1</v>
+      </c>
       <c r="BJ47" s="60"/>
-      <c r="BK47" s="60"/>
-      <c r="BL47" s="60"/>
-      <c r="BM47" s="60"/>
-      <c r="BN47" s="60"/>
+      <c r="BK47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BL47" s="106">
+        <v>1</v>
+      </c>
+      <c r="BM47" s="105">
+        <v>0</v>
+      </c>
+      <c r="BN47" s="106">
+        <v>1</v>
+      </c>
       <c r="BO47" s="60"/>
       <c r="BP47" s="60"/>
       <c r="BQ47" s="60"/>
@@ -17864,12 +17962,20 @@
       </c>
       <c r="K88" s="24"/>
       <c r="L88" s="21"/>
-      <c r="M88" s="24"/>
-      <c r="N88" s="21"/>
-      <c r="O88" s="21"/>
-      <c r="P88" s="21"/>
-      <c r="Q88" s="21"/>
-      <c r="R88" s="83"/>
+      <c r="M88" s="275" t="s">
+        <v>422</v>
+      </c>
+      <c r="N88" s="274" t="s">
+        <v>423</v>
+      </c>
+      <c r="O88" s="274"/>
+      <c r="P88" s="274"/>
+      <c r="Q88" s="274" t="s">
+        <v>424</v>
+      </c>
+      <c r="R88" s="116" t="s">
+        <v>204</v>
+      </c>
       <c r="S88" s="82" t="s">
         <v>19</v>
       </c>
@@ -17883,47 +17989,117 @@
       <c r="W88" s="68"/>
       <c r="X88" s="68"/>
       <c r="Y88" s="60"/>
-      <c r="Z88" s="60"/>
-      <c r="AA88" s="60"/>
-      <c r="AB88" s="60"/>
-      <c r="AC88" s="60"/>
-      <c r="AD88" s="60"/>
-      <c r="AE88" s="60"/>
-      <c r="AF88" s="60"/>
-      <c r="AG88" s="60"/>
-      <c r="AH88" s="60"/>
-      <c r="AI88" s="60"/>
-      <c r="AJ88" s="60"/>
-      <c r="AK88" s="60"/>
-      <c r="AL88" s="60"/>
-      <c r="AM88" s="60"/>
-      <c r="AN88" s="60"/>
-      <c r="AO88" s="60"/>
-      <c r="AP88" s="60"/>
-      <c r="AQ88" s="60"/>
-      <c r="AR88" s="60"/>
-      <c r="AS88" s="60"/>
-      <c r="AT88" s="60"/>
-      <c r="AU88" s="60"/>
-      <c r="AV88" s="60"/>
-      <c r="AW88" s="60"/>
-      <c r="AX88" s="60"/>
-      <c r="AY88" s="60"/>
-      <c r="AZ88" s="60"/>
-      <c r="BA88" s="60"/>
-      <c r="BB88" s="60"/>
-      <c r="BC88" s="60"/>
-      <c r="BD88" s="60"/>
-      <c r="BE88" s="60"/>
-      <c r="BF88" s="60"/>
-      <c r="BG88" s="60"/>
-      <c r="BH88" s="60"/>
-      <c r="BI88" s="60"/>
-      <c r="BJ88" s="60"/>
-      <c r="BK88" s="60"/>
-      <c r="BL88" s="60"/>
-      <c r="BM88" s="60"/>
-      <c r="BN88" s="60"/>
+      <c r="Z88" s="104">
+        <v>0</v>
+      </c>
+      <c r="AA88" s="130">
+        <v>1</v>
+      </c>
+      <c r="AB88" s="130">
+        <v>1</v>
+      </c>
+      <c r="AC88" s="119" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AE88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AF88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AG88" s="131" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH88" s="131"/>
+      <c r="AI88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AJ88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AK88" s="132">
+        <v>1</v>
+      </c>
+      <c r="AL88" s="120">
+        <v>1</v>
+      </c>
+      <c r="AM88" s="134" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN88" s="133">
+        <v>0</v>
+      </c>
+      <c r="AO88" s="133">
+        <v>0</v>
+      </c>
+      <c r="AP88" s="130">
+        <v>1</v>
+      </c>
+      <c r="AQ88" s="106">
+        <v>1</v>
+      </c>
+      <c r="AR88" s="106">
+        <v>1</v>
+      </c>
+      <c r="AS88" s="130">
+        <v>1</v>
+      </c>
+      <c r="AT88" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU88" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV88" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW88" s="135"/>
+      <c r="AX88" s="135"/>
+      <c r="AY88" s="130">
+        <v>1</v>
+      </c>
+      <c r="AZ88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BA88" s="136" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BC88" s="136" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD88" s="135"/>
+      <c r="BE88" s="135"/>
+      <c r="BF88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BG88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BH88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BI88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BJ88" s="135"/>
+      <c r="BK88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BL88" s="130">
+        <v>1</v>
+      </c>
+      <c r="BM88" s="137">
+        <v>0</v>
+      </c>
+      <c r="BN88" s="138">
+        <v>1</v>
+      </c>
       <c r="BO88" s="60"/>
       <c r="BP88" s="60"/>
       <c r="BQ88" s="60"/>

</xml_diff>